<commit_message>
Ticket #9524 corrected calbration sheet from Steve Gaul added to repository.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\IRAD\IRAD 2015\Programs\OOI Phase 2\Post Delivery 7 support\Asset Management Data\ingestion-csvs_20151204\ingestion-csvs\GP02HYPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Desktop\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6456" yWindow="5940" windowWidth="29604" windowHeight="14424" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16908" windowHeight="9300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="80">
   <si>
     <t>Ref Des</t>
   </si>
@@ -280,9 +280,6 @@
       </rPr>
       <t>000</t>
     </r>
-  </si>
-  <si>
-    <t>GP02HYPM-00001-GPM01</t>
   </si>
   <si>
     <t>This is a made-up serial number for the controller card</t>
@@ -408,6 +405,12 @@
   <si>
     <t>A00146</t>
   </si>
+  <si>
+    <t>GP02HYPM-00001-SIOENG</t>
+  </si>
+  <si>
+    <t>R00054</t>
+  </si>
 </sst>
 </file>
 
@@ -420,7 +423,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,7 +615,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,8 +651,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -708,6 +717,21 @@
       </top>
       <bottom style="hair">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -977,9 +1001,6 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1017,6 +1038,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="131">
     <cellStyle name="Comma 2" xfId="62"/>
@@ -1224,7 +1246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1259,7 +1281,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1474,7 +1496,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="11.77734375" style="5" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
@@ -1495,41 +1517,41 @@
     <col min="17" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="27.6">
+      <c r="A1" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="53" t="s">
         <v>31</v>
       </c>
       <c r="M1" s="25" t="s">
@@ -1545,9 +1567,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="15" customFormat="1" ht="14.4">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>42</v>
@@ -1555,31 +1577,31 @@
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="47">
-        <v>1</v>
-      </c>
-      <c r="E2" s="48">
+      <c r="D2" s="46">
+        <v>1</v>
+      </c>
+      <c r="E2" s="47">
         <v>41481</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="48">
         <v>0.34097222222222223</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G2" s="47">
         <v>41842</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="47">
+      <c r="J2" s="46">
         <v>4219</v>
       </c>
-      <c r="K2" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="53">
+      <c r="K2" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="52">
         <v>41804</v>
       </c>
       <c r="M2" s="24">
@@ -1597,7 +1619,7 @@
         <v>41593</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" s="15" customFormat="1">
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
       <c r="G3" s="20"/>
@@ -1618,17 +1640,17 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="E46:E48"/>
+      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="33.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
     <col min="5" max="5" width="12" style="7" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
@@ -1640,12 +1662,12 @@
     <col min="15" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="57" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="56" customFormat="1" ht="27.6">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
@@ -1654,22 +1676,22 @@
         <v>35</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="I1" s="55" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="12" customFormat="1">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1680,12 +1702,12 @@
       <c r="H2" s="11"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.4">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>13</v>
@@ -1693,8 +1715,8 @@
       <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E3" s="58" t="s">
-        <v>69</v>
+      <c r="E3" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F3" s="4">
         <v>2736</v>
@@ -1709,12 +1731,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.4">
       <c r="A4" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>13</v>
@@ -1722,8 +1744,8 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="58" t="s">
-        <v>69</v>
+      <c r="E4" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F4" s="22">
         <v>2736</v>
@@ -1736,12 +1758,12 @@
       </c>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.4">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>13</v>
@@ -1749,8 +1771,8 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="58" t="s">
-        <v>69</v>
+      <c r="E5" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F5" s="22">
         <v>2736</v>
@@ -1763,12 +1785,12 @@
       </c>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.4">
       <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>13</v>
@@ -1776,8 +1798,8 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="58" t="s">
-        <v>69</v>
+      <c r="E6" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F6" s="22">
         <v>2736</v>
@@ -1790,12 +1812,12 @@
       </c>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.4">
       <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>13</v>
@@ -1803,8 +1825,8 @@
       <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="58" t="s">
-        <v>69</v>
+      <c r="E7" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F7" s="22">
         <v>2736</v>
@@ -1819,12 +1841,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.4">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>13</v>
@@ -1832,8 +1854,8 @@
       <c r="D8" s="7">
         <v>1</v>
       </c>
-      <c r="E8" s="58" t="s">
-        <v>69</v>
+      <c r="E8" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F8" s="22">
         <v>2736</v>
@@ -1848,12 +1870,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.4">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>13</v>
@@ -1861,8 +1883,8 @@
       <c r="D9" s="7">
         <v>1</v>
       </c>
-      <c r="E9" s="58" t="s">
-        <v>69</v>
+      <c r="E9" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F9" s="22">
         <v>2736</v>
@@ -1870,19 +1892,19 @@
       <c r="G9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="51">
         <v>1.0960000000000001</v>
       </c>
       <c r="I9" s="36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.4">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>13</v>
@@ -1890,8 +1912,8 @@
       <c r="D10" s="7">
         <v>1</v>
       </c>
-      <c r="E10" s="58" t="s">
-        <v>69</v>
+      <c r="E10" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="F10" s="22">
         <v>2736</v>
@@ -1906,19 +1928,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="29"/>
       <c r="B11" s="40"/>
       <c r="C11" s="28"/>
       <c r="F11" s="22"/>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.4">
       <c r="A12" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>13</v>
@@ -1926,8 +1948,8 @@
       <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="58" t="s">
-        <v>70</v>
+      <c r="E12" s="57" t="s">
+        <v>69</v>
       </c>
       <c r="F12" s="4">
         <v>1086</v>
@@ -1942,12 +1964,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.4">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>13</v>
@@ -1955,8 +1977,8 @@
       <c r="D13" s="7">
         <v>1</v>
       </c>
-      <c r="E13" s="58" t="s">
-        <v>70</v>
+      <c r="E13" s="57" t="s">
+        <v>69</v>
       </c>
       <c r="F13" s="22">
         <v>1086</v>
@@ -1968,7 +1990,7 @@
         <v>-144.798</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="29"/>
       <c r="B14" s="40"/>
       <c r="C14" s="28"/>
@@ -1976,12 +1998,12 @@
       <c r="G14" s="34"/>
       <c r="H14" s="35"/>
     </row>
-    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.4">
       <c r="A15" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>13</v>
@@ -1989,8 +2011,8 @@
       <c r="D15" s="7">
         <v>1</v>
       </c>
-      <c r="E15" s="58" t="s">
-        <v>71</v>
+      <c r="E15" s="57" t="s">
+        <v>70</v>
       </c>
       <c r="F15" s="4">
         <v>107</v>
@@ -2002,12 +2024,12 @@
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.4">
       <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>13</v>
@@ -2015,8 +2037,8 @@
       <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="58" t="s">
-        <v>71</v>
+      <c r="E16" s="57" t="s">
+        <v>70</v>
       </c>
       <c r="F16" s="22">
         <v>107</v>
@@ -2028,7 +2050,7 @@
         <v>-144.798</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="29"/>
       <c r="B17" s="40"/>
       <c r="C17" s="28"/>
@@ -2036,12 +2058,12 @@
       <c r="G17" s="26"/>
       <c r="H17" s="35"/>
     </row>
-    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.4">
       <c r="A18" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>13</v>
@@ -2049,8 +2071,8 @@
       <c r="D18" s="7">
         <v>1</v>
       </c>
-      <c r="E18" s="58" t="s">
-        <v>72</v>
+      <c r="E18" s="57" t="s">
+        <v>71</v>
       </c>
       <c r="F18" s="4">
         <v>1024</v>
@@ -2062,12 +2084,12 @@
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.4">
       <c r="A19" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>13</v>
@@ -2075,8 +2097,8 @@
       <c r="D19" s="28">
         <v>1</v>
       </c>
-      <c r="E19" s="58" t="s">
-        <v>72</v>
+      <c r="E19" s="57" t="s">
+        <v>71</v>
       </c>
       <c r="F19" s="22">
         <v>1024</v>
@@ -2088,7 +2110,7 @@
         <v>-144.798</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="29"/>
       <c r="B20" s="40"/>
       <c r="C20" s="28"/>
@@ -2098,12 +2120,12 @@
       <c r="G20" s="34"/>
       <c r="H20" s="35"/>
     </row>
-    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.4">
       <c r="A21" s="42" t="s">
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="43" t="s">
         <v>13</v>
@@ -2112,16 +2134,16 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
         <v>66</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
       </c>
       <c r="G21" s="34"/>
       <c r="H21" s="35"/>
       <c r="I21" s="31"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="29"/>
       <c r="B22" s="40"/>
       <c r="C22" s="28"/>
@@ -2131,12 +2153,12 @@
       <c r="G22" s="34"/>
       <c r="H22" s="35"/>
     </row>
-    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.4">
       <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>13</v>
@@ -2144,8 +2166,8 @@
       <c r="D23" s="7">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>73</v>
+      <c r="E23" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F23" s="4">
         <v>2350</v>
@@ -2160,12 +2182,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.4">
       <c r="A24" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="28" t="s">
         <v>13</v>
@@ -2173,8 +2195,8 @@
       <c r="D24" s="7">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>73</v>
+      <c r="E24" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F24" s="22">
         <v>2350</v>
@@ -2187,12 +2209,12 @@
       </c>
       <c r="I24" s="34"/>
     </row>
-    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.4">
       <c r="A25" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>13</v>
@@ -2200,8 +2222,8 @@
       <c r="D25" s="7">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
-        <v>73</v>
+      <c r="E25" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F25" s="22">
         <v>2350</v>
@@ -2214,12 +2236,12 @@
       </c>
       <c r="I25" s="37"/>
     </row>
-    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.4">
       <c r="A26" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>13</v>
@@ -2227,8 +2249,8 @@
       <c r="D26" s="7">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>73</v>
+      <c r="E26" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F26" s="22">
         <v>2350</v>
@@ -2241,12 +2263,12 @@
       </c>
       <c r="I26" s="37"/>
     </row>
-    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.4">
       <c r="A27" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>13</v>
@@ -2254,8 +2276,8 @@
       <c r="D27" s="7">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
-        <v>73</v>
+      <c r="E27" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F27" s="22">
         <v>2350</v>
@@ -2270,12 +2292,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.4">
       <c r="A28" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>13</v>
@@ -2283,8 +2305,8 @@
       <c r="D28" s="7">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>73</v>
+      <c r="E28" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F28" s="22">
         <v>2350</v>
@@ -2299,12 +2321,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14.4">
       <c r="A29" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>13</v>
@@ -2312,8 +2334,8 @@
       <c r="D29" s="7">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>73</v>
+      <c r="E29" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F29" s="22">
         <v>2350</v>
@@ -2321,19 +2343,19 @@
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="52">
+      <c r="H29" s="51">
         <v>1.0960000000000001</v>
       </c>
       <c r="I29" s="36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.4">
       <c r="A30" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>13</v>
@@ -2341,8 +2363,8 @@
       <c r="D30" s="7">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
-        <v>73</v>
+      <c r="E30" s="58" t="s">
+        <v>72</v>
       </c>
       <c r="F30" s="22">
         <v>2350</v>
@@ -2357,19 +2379,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="29"/>
       <c r="B31" s="40"/>
       <c r="C31" s="28"/>
       <c r="F31" s="22"/>
       <c r="I31" s="36"/>
     </row>
-    <row r="32" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14.4">
       <c r="A32" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>13</v>
@@ -2377,8 +2399,8 @@
       <c r="D32" s="7">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
-        <v>74</v>
+      <c r="E32" s="58" t="s">
+        <v>73</v>
       </c>
       <c r="F32" s="4">
         <v>1106</v>
@@ -2390,12 +2412,12 @@
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="14.4">
       <c r="A33" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>13</v>
@@ -2403,8 +2425,8 @@
       <c r="D33" s="7">
         <v>1</v>
       </c>
-      <c r="E33" t="s">
-        <v>74</v>
+      <c r="E33" s="58" t="s">
+        <v>73</v>
       </c>
       <c r="F33" s="22">
         <v>1106</v>
@@ -2416,7 +2438,7 @@
         <v>-144.798</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="29"/>
       <c r="B34" s="40"/>
       <c r="C34" s="28"/>
@@ -2424,12 +2446,12 @@
       <c r="G34" s="34"/>
       <c r="H34" s="33"/>
     </row>
-    <row r="35" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="14.4">
       <c r="A35" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>13</v>
@@ -2437,8 +2459,8 @@
       <c r="D35" s="7">
         <v>1</v>
       </c>
-      <c r="E35" t="s">
-        <v>75</v>
+      <c r="E35" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="F35" s="4">
         <v>97</v>
@@ -2450,12 +2472,12 @@
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="14.4">
       <c r="A36" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>13</v>
@@ -2463,8 +2485,8 @@
       <c r="D36" s="7">
         <v>1</v>
       </c>
-      <c r="E36" t="s">
-        <v>75</v>
+      <c r="E36" s="58" t="s">
+        <v>74</v>
       </c>
       <c r="F36" s="22">
         <v>97</v>
@@ -2476,7 +2498,7 @@
         <v>-144.798</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13">
       <c r="A37" s="29"/>
       <c r="B37" s="40"/>
       <c r="C37" s="28"/>
@@ -2484,12 +2506,12 @@
       <c r="G37" s="26"/>
       <c r="H37" s="35"/>
     </row>
-    <row r="38" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="14.4">
       <c r="A38" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>13</v>
@@ -2497,8 +2519,8 @@
       <c r="D38" s="7">
         <v>1</v>
       </c>
-      <c r="E38" t="s">
-        <v>76</v>
+      <c r="E38" s="58" t="s">
+        <v>75</v>
       </c>
       <c r="F38" s="4">
         <v>1025</v>
@@ -2510,12 +2532,12 @@
         <v>50.070666666666703</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="14.4">
       <c r="A39" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" s="28" t="s">
         <v>13</v>
@@ -2523,8 +2545,8 @@
       <c r="D39" s="28">
         <v>1</v>
       </c>
-      <c r="E39" t="s">
-        <v>76</v>
+      <c r="E39" s="58" t="s">
+        <v>75</v>
       </c>
       <c r="F39" s="22">
         <v>1025</v>
@@ -2536,7 +2558,7 @@
         <v>-144.798</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13">
       <c r="A40" s="40"/>
       <c r="B40" s="40"/>
       <c r="C40" s="28"/>
@@ -2546,12 +2568,12 @@
       <c r="G40" s="34"/>
       <c r="H40" s="33"/>
     </row>
-    <row r="41" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="14.4">
       <c r="A41" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="43" t="s">
         <v>13</v>
@@ -2560,10 +2582,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G41" s="34"/>
       <c r="H41" s="33"/>
@@ -2573,7 +2595,7 @@
       <c r="L41" s="31"/>
       <c r="M41" s="31"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13">
       <c r="A42" s="29"/>
       <c r="B42" s="40"/>
       <c r="C42" s="28"/>
@@ -2588,12 +2610,12 @@
       <c r="L42" s="31"/>
       <c r="M42" s="31"/>
     </row>
-    <row r="43" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="51" t="s">
-        <v>60</v>
+    <row r="43" spans="1:13" ht="14.4">
+      <c r="A43" s="50" t="s">
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
@@ -2609,12 +2631,12 @@
       <c r="L43" s="31"/>
       <c r="M43" s="31"/>
     </row>
-    <row r="44" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="51" t="s">
-        <v>61</v>
+    <row r="44" spans="1:13" ht="14.4">
+      <c r="A44" s="50" t="s">
+        <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
@@ -2630,7 +2652,7 @@
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13">
       <c r="A45" s="40"/>
       <c r="B45" s="40"/>
       <c r="C45" s="28"/>
@@ -2645,12 +2667,12 @@
       <c r="L45" s="31"/>
       <c r="M45" s="31"/>
     </row>
-    <row r="46" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" ht="14.4">
       <c r="A46" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>13</v>
@@ -2659,27 +2681,27 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="46">
+      <c r="H46" s="45">
         <v>1450</v>
       </c>
       <c r="I46" s="31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="14.55" customHeight="1">
       <c r="A47" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" s="28" t="s">
         <v>13</v>
@@ -2688,10 +2710,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
@@ -2700,12 +2722,12 @@
         <v>50.070666666666668</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="14.55" customHeight="1">
       <c r="A48" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="28" t="s">
         <v>13</v>
@@ -2714,10 +2736,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G48" s="27" t="s">
         <v>16</v>
@@ -2726,12 +2748,12 @@
         <v>-144.798</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="14.4">
       <c r="A50" s="42" t="s">
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="43" t="s">
         <v>13</v>
@@ -2739,12 +2761,14 @@
       <c r="D50" s="44">
         <v>1</v>
       </c>
-      <c r="E50" s="44"/>
-      <c r="F50" s="45" t="s">
+      <c r="E50" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50" s="31" t="s">
         <v>54</v>
-      </c>
-      <c r="I50" s="31" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected CTDMO to nominal reference designator
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16905" windowHeight="9300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16905" windowHeight="9300"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="78">
   <si>
     <t>Ref Des</t>
   </si>
@@ -240,67 +240,6 @@
     <t>This is a made-up serial number for the controller card</t>
   </si>
   <si>
-    <r>
-      <t>GP02HYPM-RI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>01-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>02</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-CTDMOG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>061</t>
-    </r>
-  </si>
-  <si>
-    <t>GP02HYPM-RIM01-02-CTDMOG061</t>
-  </si>
-  <si>
-    <t>Nominal imodem ID is 39, but actual for this deployment is 61</t>
-  </si>
-  <si>
     <t>MV-130</t>
   </si>
   <si>
@@ -368,6 +307,9 @@
   </si>
   <si>
     <t>GP02HYPM-RIM01-00-SIOENG000</t>
+  </si>
+  <si>
+    <t>GP02HYPM-RIM01-02-CTDMOG039</t>
   </si>
 </sst>
 </file>
@@ -1451,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1420,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B1" s="53" t="s">
         <v>0</v>
@@ -1528,7 +1470,7 @@
     </row>
     <row r="2" spans="1:16" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>42</v>
@@ -1558,7 +1500,7 @@
         <v>4219</v>
       </c>
       <c r="K2" s="49" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" s="52">
         <v>41804</v>
@@ -1596,13 +1538,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B57" sqref="B57"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1615,18 +1557,19 @@
     <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="10.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="10.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="56" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="56" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
@@ -1635,7 +1578,7 @@
         <v>35</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>2</v>
@@ -1650,7 +1593,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1660,13 +1603,14 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>13</v>
@@ -1675,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4">
         <v>2736</v>
@@ -1689,13 +1633,15 @@
       <c r="I3" s="37" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K3" s="12"/>
+      <c r="P3" s="12"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>13</v>
@@ -1704,7 +1650,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" s="22">
         <v>2736</v>
@@ -1716,13 +1662,15 @@
         <v>1.871E-6</v>
       </c>
       <c r="I4" s="37"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K4" s="12"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>13</v>
@@ -1731,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" s="22">
         <v>2736</v>
@@ -1743,13 +1691,15 @@
         <v>52</v>
       </c>
       <c r="I5" s="37"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K5" s="12"/>
+      <c r="P5" s="12"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>13</v>
@@ -1758,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F6" s="22">
         <v>2736</v>
@@ -1770,13 +1720,15 @@
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="I6" s="37"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K6" s="12"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>13</v>
@@ -1785,7 +1737,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F7" s="22">
         <v>2736</v>
@@ -1799,13 +1751,15 @@
       <c r="I7" s="36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K7" s="12"/>
+      <c r="P7" s="12"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>13</v>
@@ -1814,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F8" s="22">
         <v>2736</v>
@@ -1828,13 +1782,15 @@
       <c r="I8" s="36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K8" s="12"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>13</v>
@@ -1843,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F9" s="22">
         <v>2736</v>
@@ -1857,13 +1813,15 @@
       <c r="I9" s="36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K9" s="12"/>
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>13</v>
@@ -1872,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F10" s="22">
         <v>2736</v>
@@ -1886,20 +1844,24 @@
       <c r="I10" s="36" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" s="12"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
       <c r="B11" s="40"/>
       <c r="C11" s="28"/>
       <c r="F11" s="22"/>
       <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K11" s="12"/>
+      <c r="P11" s="12"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>13</v>
@@ -1908,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F12" s="4">
         <v>1086</v>
@@ -1922,13 +1884,15 @@
       <c r="I12" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K12" s="12"/>
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>13</v>
@@ -1937,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F13" s="22">
         <v>1086</v>
@@ -1948,21 +1912,25 @@
       <c r="H13" s="35">
         <v>-144.798</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K13" s="12"/>
+      <c r="P13" s="12"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
       <c r="B14" s="40"/>
       <c r="C14" s="28"/>
       <c r="F14" s="22"/>
       <c r="G14" s="34"/>
       <c r="H14" s="35"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K14" s="12"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>13</v>
@@ -1971,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" s="4">
         <v>107</v>
@@ -1982,13 +1950,15 @@
       <c r="H15" s="35">
         <v>50.070666666666668</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K15" s="12"/>
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>13</v>
@@ -1997,7 +1967,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16" s="22">
         <v>107</v>
@@ -2008,21 +1978,23 @@
       <c r="H16" s="35">
         <v>-144.798</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="40"/>
       <c r="C17" s="28"/>
       <c r="F17" s="22"/>
       <c r="G17" s="26"/>
       <c r="H17" s="35"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>13</v>
@@ -2031,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F18" s="4">
         <v>1024</v>
@@ -2042,13 +2014,14 @@
       <c r="H18" s="35">
         <v>50.070666666666668</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>13</v>
@@ -2057,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F19" s="22">
         <v>1024</v>
@@ -2068,8 +2041,9 @@
       <c r="H19" s="35">
         <v>-144.798</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
       <c r="B20" s="40"/>
       <c r="C20" s="28"/>
@@ -2078,31 +2052,33 @@
       <c r="F20" s="22"/>
       <c r="G20" s="34"/>
       <c r="H20" s="35"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>51</v>
       </c>
       <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="44">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="44">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G21" s="34"/>
       <c r="H21" s="35"/>
       <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="40"/>
       <c r="C22" s="28"/>
@@ -2111,13 +2087,14 @@
       <c r="F22" s="22"/>
       <c r="G22" s="34"/>
       <c r="H22" s="35"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>13</v>
@@ -2126,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" s="4">
         <v>2350</v>
@@ -2140,13 +2117,14 @@
       <c r="I23" s="37" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C24" s="28" t="s">
         <v>13</v>
@@ -2155,7 +2133,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F24" s="22">
         <v>2350</v>
@@ -2167,13 +2145,14 @@
         <v>2.0339999999999999E-6</v>
       </c>
       <c r="I24" s="34"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>13</v>
@@ -2182,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F25" s="22">
         <v>2350</v>
@@ -2194,13 +2173,14 @@
         <v>48</v>
       </c>
       <c r="I25" s="37"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>13</v>
@@ -2209,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F26" s="22">
         <v>2350</v>
@@ -2221,13 +2201,14 @@
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="I26" s="37"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>13</v>
@@ -2236,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F27" s="22">
         <v>2350</v>
@@ -2250,13 +2231,14 @@
       <c r="I27" s="36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>13</v>
@@ -2265,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F28" s="22">
         <v>2350</v>
@@ -2279,13 +2261,14 @@
       <c r="I28" s="36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>13</v>
@@ -2294,7 +2277,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F29" s="22">
         <v>2350</v>
@@ -2308,13 +2291,14 @@
       <c r="I29" s="36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>13</v>
@@ -2323,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F30" s="22">
         <v>2350</v>
@@ -2337,20 +2321,22 @@
       <c r="I30" s="36" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="40"/>
       <c r="C31" s="28"/>
       <c r="F31" s="22"/>
       <c r="I31" s="36"/>
-    </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>13</v>
@@ -2359,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F32" s="4">
         <v>1106</v>
@@ -2370,13 +2356,14 @@
       <c r="H32" s="33">
         <v>50.070666666666668</v>
       </c>
+      <c r="K32" s="12"/>
     </row>
     <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>13</v>
@@ -2385,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F33" s="22">
         <v>1106</v>
@@ -2396,6 +2383,7 @@
       <c r="H33" s="33">
         <v>-144.798</v>
       </c>
+      <c r="K33" s="12"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
@@ -2404,13 +2392,14 @@
       <c r="F34" s="22"/>
       <c r="G34" s="34"/>
       <c r="H34" s="33"/>
+      <c r="K34" s="12"/>
     </row>
     <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>13</v>
@@ -2419,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F35" s="4">
         <v>97</v>
@@ -2430,13 +2419,14 @@
       <c r="H35" s="35">
         <v>50.070666666666668</v>
       </c>
+      <c r="K35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>13</v>
@@ -2445,7 +2435,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F36" s="22">
         <v>97</v>
@@ -2456,6 +2446,7 @@
       <c r="H36" s="35">
         <v>-144.798</v>
       </c>
+      <c r="K36" s="12"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="29"/>
@@ -2464,13 +2455,14 @@
       <c r="F37" s="22"/>
       <c r="G37" s="26"/>
       <c r="H37" s="35"/>
+      <c r="K37" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>13</v>
@@ -2479,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="58" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F38" s="4">
         <v>1025</v>
@@ -2490,13 +2482,14 @@
       <c r="H38" s="33">
         <v>50.070666666666703</v>
       </c>
+      <c r="K38" s="12"/>
     </row>
     <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C39" s="28" t="s">
         <v>13</v>
@@ -2505,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F39" s="22">
         <v>1025</v>
@@ -2516,6 +2509,7 @@
       <c r="H39" s="33">
         <v>-144.798</v>
       </c>
+      <c r="K39" s="12"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
@@ -2526,13 +2520,14 @@
       <c r="F40" s="22"/>
       <c r="G40" s="34"/>
       <c r="H40" s="33"/>
+      <c r="K40" s="12"/>
     </row>
     <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C41" s="43" t="s">
         <v>13</v>
@@ -2541,16 +2536,16 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" t="s">
         <v>63</v>
-      </c>
-      <c r="F41" t="s">
-        <v>66</v>
       </c>
       <c r="G41" s="34"/>
       <c r="H41" s="33"/>
       <c r="I41" s="31"/>
       <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
+      <c r="K41" s="12"/>
       <c r="L41" s="31"/>
       <c r="M41" s="31"/>
     </row>
@@ -2565,16 +2560,16 @@
       <c r="H42" s="33"/>
       <c r="I42" s="32"/>
       <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
+      <c r="K42" s="12"/>
       <c r="L42" s="31"/>
       <c r="M42" s="31"/>
     </row>
     <row r="43" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
@@ -2586,16 +2581,16 @@
         <v>49</v>
       </c>
       <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
+      <c r="K43" s="12"/>
       <c r="L43" s="31"/>
       <c r="M43" s="31"/>
     </row>
     <row r="44" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
@@ -2607,7 +2602,7 @@
         <v>50</v>
       </c>
       <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
+      <c r="K44" s="12"/>
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
     </row>
@@ -2622,16 +2617,16 @@
       <c r="H45" s="33"/>
       <c r="I45" s="39"/>
       <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
+      <c r="K45" s="12"/>
       <c r="L45" s="31"/>
       <c r="M45" s="31"/>
     </row>
     <row r="46" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="42" t="s">
-        <v>54</v>
+      <c r="A46" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>13</v>
@@ -2640,10 +2635,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>14</v>
@@ -2651,16 +2646,15 @@
       <c r="H46" s="45">
         <v>1450</v>
       </c>
-      <c r="I46" s="31" t="s">
-        <v>56</v>
-      </c>
+      <c r="I46" s="31"/>
+      <c r="K46" s="12"/>
     </row>
     <row r="47" spans="1:13" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
-        <v>55</v>
+      <c r="A47" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C47" s="28" t="s">
         <v>13</v>
@@ -2669,10 +2663,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F47" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>15</v>
@@ -2680,13 +2674,14 @@
       <c r="H47" s="26">
         <v>50.070666666666668</v>
       </c>
+      <c r="K47" s="12"/>
     </row>
     <row r="48" spans="1:13" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
-        <v>55</v>
+      <c r="A48" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C48" s="28" t="s">
         <v>13</v>
@@ -2695,10 +2690,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F48" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G48" s="27" t="s">
         <v>16</v>
@@ -2706,13 +2701,17 @@
       <c r="H48" s="26">
         <v>-144.798</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="12"/>
+    </row>
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="59" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C50" s="43" t="s">
         <v>13</v>
@@ -2721,14 +2720,21 @@
         <v>1</v>
       </c>
       <c r="E50" s="58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F50" s="58" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I50" s="31" t="s">
         <v>53</v>
       </c>
+      <c r="K50" s="12"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="12"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Global Papa - fixed deployment dates
Fixed deployment dates based on cruise reports and WHOI documentation
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16905" windowHeight="9300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29420" windowHeight="13700"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1088,7 +1083,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1147,7 +1142,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1182,7 +1177,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1394,31 +1389,31 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="5"/>
-    <col min="16" max="16" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.7109375" style="5"/>
+    <col min="1" max="1" width="11.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" style="5"/>
+    <col min="16" max="16" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="28">
       <c r="A1" s="53" t="s">
         <v>57</v>
       </c>
@@ -1468,7 +1463,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="15" customFormat="1">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1488,7 +1483,7 @@
         <v>0.34097222222222223</v>
       </c>
       <c r="G2" s="47">
-        <v>41842</v>
+        <v>41804</v>
       </c>
       <c r="H2" s="46" t="s">
         <v>41</v>
@@ -1520,7 +1515,7 @@
         <v>41593</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="15" customFormat="1">
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
       <c r="G3" s="20"/>
@@ -1547,24 +1542,24 @@
       <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
     <col min="5" max="5" width="12" style="7" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="1" customWidth="1"/>
-    <col min="11" max="13" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="1" customWidth="1"/>
+    <col min="11" max="13" width="10.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.7109375" style="1"/>
+    <col min="15" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="56" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="56" customFormat="1" ht="28">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1588,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="12" customFormat="1">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1605,7 +1600,7 @@
       <c r="I2" s="13"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -1636,7 +1631,7 @@
       <c r="K3" s="12"/>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="29" t="s">
         <v>5</v>
       </c>
@@ -1665,7 +1660,7 @@
       <c r="K4" s="12"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -1694,7 +1689,7 @@
       <c r="K5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1718,7 @@
       <c r="K6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
@@ -1754,7 +1749,7 @@
       <c r="K7" s="12"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -1785,7 +1780,7 @@
       <c r="K8" s="12"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
@@ -1816,7 +1811,7 @@
       <c r="K9" s="12"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
@@ -1847,7 +1842,7 @@
       <c r="K10" s="12"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="29"/>
       <c r="B11" s="40"/>
       <c r="C11" s="28"/>
@@ -1856,7 +1851,7 @@
       <c r="K11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="30" t="s">
         <v>6</v>
       </c>
@@ -1887,7 +1882,7 @@
       <c r="K12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1910,7 @@
       <c r="K13" s="12"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="29"/>
       <c r="B14" s="40"/>
       <c r="C14" s="28"/>
@@ -1925,7 +1920,7 @@
       <c r="K14" s="12"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="30" t="s">
         <v>7</v>
       </c>
@@ -1953,7 +1948,7 @@
       <c r="K15" s="12"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
@@ -1980,7 +1975,7 @@
       </c>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="29"/>
       <c r="B17" s="40"/>
       <c r="C17" s="28"/>
@@ -1989,7 +1984,7 @@
       <c r="H17" s="35"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="30" t="s">
         <v>8</v>
       </c>
@@ -2016,7 +2011,7 @@
       </c>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="29" t="s">
         <v>8</v>
       </c>
@@ -2043,7 +2038,7 @@
       </c>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="29"/>
       <c r="B20" s="40"/>
       <c r="C20" s="28"/>
@@ -2054,7 +2049,7 @@
       <c r="H20" s="35"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="42" t="s">
         <v>51</v>
       </c>
@@ -2078,7 +2073,7 @@
       <c r="I21" s="31"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="29"/>
       <c r="B22" s="40"/>
       <c r="C22" s="28"/>
@@ -2089,7 +2084,7 @@
       <c r="H22" s="35"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
@@ -2119,7 +2114,7 @@
       </c>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="29" t="s">
         <v>9</v>
       </c>
@@ -2147,7 +2142,7 @@
       <c r="I24" s="34"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="29" t="s">
         <v>9</v>
       </c>
@@ -2175,7 +2170,7 @@
       <c r="I25" s="37"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="29" t="s">
         <v>9</v>
       </c>
@@ -2203,7 +2198,7 @@
       <c r="I26" s="37"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="29" t="s">
         <v>9</v>
       </c>
@@ -2233,7 +2228,7 @@
       </c>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="29" t="s">
         <v>9</v>
       </c>
@@ -2263,7 +2258,7 @@
       </c>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="29" t="s">
         <v>9</v>
       </c>
@@ -2293,7 +2288,7 @@
       </c>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="29" t="s">
         <v>9</v>
       </c>
@@ -2323,7 +2318,7 @@
       </c>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="29"/>
       <c r="B31" s="40"/>
       <c r="C31" s="28"/>
@@ -2331,7 +2326,7 @@
       <c r="I31" s="36"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="30" t="s">
         <v>10</v>
       </c>
@@ -2358,7 +2353,7 @@
       </c>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" s="29" t="s">
         <v>10</v>
       </c>
@@ -2385,7 +2380,7 @@
       </c>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="29"/>
       <c r="B34" s="40"/>
       <c r="C34" s="28"/>
@@ -2394,7 +2389,7 @@
       <c r="H34" s="33"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" s="30" t="s">
         <v>11</v>
       </c>
@@ -2421,7 +2416,7 @@
       </c>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="29" t="s">
         <v>11</v>
       </c>
@@ -2448,7 +2443,7 @@
       </c>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="29"/>
       <c r="B37" s="40"/>
       <c r="C37" s="28"/>
@@ -2457,7 +2452,7 @@
       <c r="H37" s="35"/>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="30" t="s">
         <v>12</v>
       </c>
@@ -2484,7 +2479,7 @@
       </c>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" s="29" t="s">
         <v>12</v>
       </c>
@@ -2511,7 +2506,7 @@
       </c>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" s="40"/>
       <c r="B40" s="40"/>
       <c r="C40" s="28"/>
@@ -2522,7 +2517,7 @@
       <c r="H40" s="33"/>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" s="42" t="s">
         <v>52</v>
       </c>
@@ -2549,7 +2544,7 @@
       <c r="L41" s="31"/>
       <c r="M41" s="31"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" s="29"/>
       <c r="B42" s="40"/>
       <c r="C42" s="28"/>
@@ -2564,7 +2559,7 @@
       <c r="L42" s="31"/>
       <c r="M42" s="31"/>
     </row>
-    <row r="43" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" s="50" t="s">
         <v>55</v>
       </c>
@@ -2585,7 +2580,7 @@
       <c r="L43" s="31"/>
       <c r="M43" s="31"/>
     </row>
-    <row r="44" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" s="50" t="s">
         <v>56</v>
       </c>
@@ -2606,7 +2601,7 @@
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" s="40"/>
       <c r="B45" s="40"/>
       <c r="C45" s="28"/>
@@ -2621,7 +2616,7 @@
       <c r="L45" s="31"/>
       <c r="M45" s="31"/>
     </row>
-    <row r="46" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
         <v>77</v>
       </c>
@@ -2649,7 +2644,7 @@
       <c r="I46" s="31"/>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="1:13" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="14.75" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>77</v>
       </c>
@@ -2676,7 +2671,7 @@
       </c>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="1:13" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="14.75" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>77</v>
       </c>
@@ -2703,10 +2698,10 @@
       </c>
       <c r="K48" s="12"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="K49" s="12"/>
     </row>
-    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" s="59" t="s">
         <v>76</v>
       </c>
@@ -2730,10 +2725,10 @@
       </c>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="K51" s="12"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="K52" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Papa CTDMO calibration coefficients
The following calibration coefficients added to all Papa CTDMOs per
Redmine ticket 10208. Updates made by Rebecca Travis.

CC_wbotc
CC_a0
CC_a1
CC_a2
CC_a3
CC_ptempa0
CC_ptempa1
CC_ptempa2
CC_ptca0
CC_ptca1
CC_ptca2
CC_ptcb0
CC_ptcb1
CC_ptcb2
CC_pa0
CC_pa1
CC_pa2
CC_g
CC_h
CC_i
CC_j
CC_cpcor
CC_ctcor
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GP02HYPM_00001.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtravis\Desktop\Cal Sheet project\Papa_cal_sheets_RT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29420" windowHeight="13700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29424" windowHeight="13704" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="103">
   <si>
     <t>Ref Des</t>
   </si>
@@ -306,19 +311,95 @@
   <si>
     <t>GP02HYPM-RIM01-02-CTDMOG039</t>
   </si>
+  <si>
+    <t>Induction ID</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>CC_wbotc</t>
+  </si>
+  <si>
+    <t>CC_a0</t>
+  </si>
+  <si>
+    <t>CC_a1</t>
+  </si>
+  <si>
+    <t>CC_a2</t>
+  </si>
+  <si>
+    <t>CC_a3</t>
+  </si>
+  <si>
+    <t>CC_ptempa0</t>
+  </si>
+  <si>
+    <t>CC_ptempa1</t>
+  </si>
+  <si>
+    <t>CC_ptempa2</t>
+  </si>
+  <si>
+    <t>CC_ptca0</t>
+  </si>
+  <si>
+    <t>CC_ptca1</t>
+  </si>
+  <si>
+    <t>CC_ptca2</t>
+  </si>
+  <si>
+    <t>CC_ptcb0</t>
+  </si>
+  <si>
+    <t>CC_ptcb1</t>
+  </si>
+  <si>
+    <t>CC_ptcb2</t>
+  </si>
+  <si>
+    <t>CC_pa0</t>
+  </si>
+  <si>
+    <t>CC_pa1</t>
+  </si>
+  <si>
+    <t>CC_pa2</t>
+  </si>
+  <si>
+    <t>CC_g</t>
+  </si>
+  <si>
+    <t>CC_h</t>
+  </si>
+  <si>
+    <t>CC_i</t>
+  </si>
+  <si>
+    <t>CC_j</t>
+  </si>
+  <si>
+    <t>CC_cpcor</t>
+  </si>
+  <si>
+    <t>CC_ctcor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,8 +590,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +636,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -764,7 +857,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -896,9 +989,6 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -935,6 +1025,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="8" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="131">
     <cellStyle name="Comma 2" xfId="62"/>
@@ -1083,7 +1194,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1388,66 +1499,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" style="5" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" style="5" customWidth="1"/>
     <col min="15" max="15" width="8.6640625" style="5"/>
     <col min="16" max="16" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="28">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="52" t="s">
         <v>31</v>
       </c>
       <c r="M1" s="25" t="s">
@@ -1463,7 +1574,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="15" customFormat="1">
+    <row r="2" spans="1:16" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1473,31 +1584,31 @@
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="46">
-        <v>1</v>
-      </c>
-      <c r="E2" s="47">
+      <c r="D2" s="45">
+        <v>1</v>
+      </c>
+      <c r="E2" s="46">
         <v>41481</v>
       </c>
-      <c r="F2" s="48">
+      <c r="F2" s="47">
         <v>0.34097222222222223</v>
       </c>
-      <c r="G2" s="47">
+      <c r="G2" s="46">
         <v>41804</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="46">
+      <c r="J2" s="45">
         <v>4219</v>
       </c>
-      <c r="K2" s="49" t="s">
+      <c r="K2" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="52">
+      <c r="L2" s="51">
         <v>41804</v>
       </c>
       <c r="M2" s="24">
@@ -1515,7 +1626,7 @@
         <v>41593</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="15" customFormat="1">
+    <row r="3" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
       <c r="G3" s="20"/>
@@ -1533,33 +1644,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" customWidth="1"/>
     <col min="5" max="5" width="12" style="7" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" style="1" customWidth="1"/>
     <col min="11" max="13" width="10.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="56" customFormat="1" ht="28">
+    <row r="1" spans="1:16" s="55" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1578,17 +1689,17 @@
       <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="12" customFormat="1">
+    <row r="2" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1600,7 +1711,7 @@
       <c r="I2" s="13"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>5</v>
       </c>
@@ -1613,7 +1724,7 @@
       <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F3" s="4">
@@ -1631,7 +1742,7 @@
       <c r="K3" s="12"/>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>5</v>
       </c>
@@ -1644,7 +1755,7 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F4" s="22">
@@ -1660,7 +1771,7 @@
       <c r="K4" s="12"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -1673,7 +1784,7 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="22">
@@ -1689,7 +1800,7 @@
       <c r="K5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
@@ -1702,7 +1813,7 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F6" s="22">
@@ -1718,7 +1829,7 @@
       <c r="K6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
@@ -1731,7 +1842,7 @@
       <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F7" s="22">
@@ -1749,7 +1860,7 @@
       <c r="K7" s="12"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -1762,7 +1873,7 @@
       <c r="D8" s="7">
         <v>1</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F8" s="22">
@@ -1780,7 +1891,7 @@
       <c r="K8" s="12"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
@@ -1793,7 +1904,7 @@
       <c r="D9" s="7">
         <v>1</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F9" s="22">
@@ -1802,7 +1913,7 @@
       <c r="G9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="50">
         <v>1.0960000000000001</v>
       </c>
       <c r="I9" s="36" t="s">
@@ -1811,7 +1922,7 @@
       <c r="K9" s="12"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
@@ -1824,7 +1935,7 @@
       <c r="D10" s="7">
         <v>1</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="56" t="s">
         <v>64</v>
       </c>
       <c r="F10" s="22">
@@ -1842,7 +1953,7 @@
       <c r="K10" s="12"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
       <c r="B11" s="40"/>
       <c r="C11" s="28"/>
@@ -1851,7 +1962,7 @@
       <c r="K11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>6</v>
       </c>
@@ -1864,7 +1975,7 @@
       <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="56" t="s">
         <v>65</v>
       </c>
       <c r="F12" s="4">
@@ -1882,7 +1993,7 @@
       <c r="K12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
@@ -1895,7 +2006,7 @@
       <c r="D13" s="7">
         <v>1</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="56" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="22">
@@ -1910,7 +2021,7 @@
       <c r="K13" s="12"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
       <c r="B14" s="40"/>
       <c r="C14" s="28"/>
@@ -1920,7 +2031,7 @@
       <c r="K14" s="12"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>7</v>
       </c>
@@ -1933,7 +2044,7 @@
       <c r="D15" s="7">
         <v>1</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="56" t="s">
         <v>66</v>
       </c>
       <c r="F15" s="4">
@@ -1948,7 +2059,7 @@
       <c r="K15" s="12"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
@@ -1961,7 +2072,7 @@
       <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="57" t="s">
+      <c r="E16" s="56" t="s">
         <v>66</v>
       </c>
       <c r="F16" s="22">
@@ -1975,7 +2086,7 @@
       </c>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="40"/>
       <c r="C17" s="28"/>
@@ -1984,7 +2095,7 @@
       <c r="H17" s="35"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>8</v>
       </c>
@@ -1997,7 +2108,7 @@
       <c r="D18" s="7">
         <v>1</v>
       </c>
-      <c r="E18" s="57" t="s">
+      <c r="E18" s="56" t="s">
         <v>67</v>
       </c>
       <c r="F18" s="4">
@@ -2011,7 +2122,7 @@
       </c>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>8</v>
       </c>
@@ -2024,7 +2135,7 @@
       <c r="D19" s="28">
         <v>1</v>
       </c>
-      <c r="E19" s="57" t="s">
+      <c r="E19" s="56" t="s">
         <v>67</v>
       </c>
       <c r="F19" s="22">
@@ -2038,7 +2149,7 @@
       </c>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="29"/>
       <c r="B20" s="40"/>
       <c r="C20" s="28"/>
@@ -2049,7 +2160,7 @@
       <c r="H20" s="35"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="42" t="s">
         <v>51</v>
       </c>
@@ -2073,7 +2184,7 @@
       <c r="I21" s="31"/>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
       <c r="B22" s="40"/>
       <c r="C22" s="28"/>
@@ -2084,7 +2195,7 @@
       <c r="H22" s="35"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
@@ -2097,7 +2208,7 @@
       <c r="D23" s="7">
         <v>1</v>
       </c>
-      <c r="E23" s="58" t="s">
+      <c r="E23" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F23" s="4">
@@ -2114,7 +2225,7 @@
       </c>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
         <v>9</v>
       </c>
@@ -2127,7 +2238,7 @@
       <c r="D24" s="7">
         <v>1</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F24" s="22">
@@ -2142,7 +2253,7 @@
       <c r="I24" s="34"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>9</v>
       </c>
@@ -2155,7 +2266,7 @@
       <c r="D25" s="7">
         <v>1</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F25" s="22">
@@ -2170,7 +2281,7 @@
       <c r="I25" s="37"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
         <v>9</v>
       </c>
@@ -2183,7 +2294,7 @@
       <c r="D26" s="7">
         <v>1</v>
       </c>
-      <c r="E26" s="58" t="s">
+      <c r="E26" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F26" s="22">
@@ -2198,7 +2309,7 @@
       <c r="I26" s="37"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>9</v>
       </c>
@@ -2211,7 +2322,7 @@
       <c r="D27" s="7">
         <v>1</v>
       </c>
-      <c r="E27" s="58" t="s">
+      <c r="E27" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F27" s="22">
@@ -2228,7 +2339,7 @@
       </c>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
         <v>9</v>
       </c>
@@ -2241,7 +2352,7 @@
       <c r="D28" s="7">
         <v>1</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F28" s="22">
@@ -2258,7 +2369,7 @@
       </c>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
         <v>9</v>
       </c>
@@ -2271,7 +2382,7 @@
       <c r="D29" s="7">
         <v>1</v>
       </c>
-      <c r="E29" s="58" t="s">
+      <c r="E29" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F29" s="22">
@@ -2280,7 +2391,7 @@
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="51">
+      <c r="H29" s="50">
         <v>1.0960000000000001</v>
       </c>
       <c r="I29" s="36" t="s">
@@ -2288,7 +2399,7 @@
       </c>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
         <v>9</v>
       </c>
@@ -2301,7 +2412,7 @@
       <c r="D30" s="7">
         <v>1</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="57" t="s">
         <v>68</v>
       </c>
       <c r="F30" s="22">
@@ -2318,7 +2429,7 @@
       </c>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="40"/>
       <c r="C31" s="28"/>
@@ -2326,7 +2437,7 @@
       <c r="I31" s="36"/>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>10</v>
       </c>
@@ -2339,7 +2450,7 @@
       <c r="D32" s="7">
         <v>1</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="57" t="s">
         <v>69</v>
       </c>
       <c r="F32" s="4">
@@ -2353,7 +2464,7 @@
       </c>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
         <v>10</v>
       </c>
@@ -2366,7 +2477,7 @@
       <c r="D33" s="7">
         <v>1</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="57" t="s">
         <v>69</v>
       </c>
       <c r="F33" s="22">
@@ -2380,7 +2491,7 @@
       </c>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
       <c r="B34" s="40"/>
       <c r="C34" s="28"/>
@@ -2389,7 +2500,7 @@
       <c r="H34" s="33"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
         <v>11</v>
       </c>
@@ -2402,7 +2513,7 @@
       <c r="D35" s="7">
         <v>1</v>
       </c>
-      <c r="E35" s="58" t="s">
+      <c r="E35" s="57" t="s">
         <v>70</v>
       </c>
       <c r="F35" s="4">
@@ -2416,7 +2527,7 @@
       </c>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
         <v>11</v>
       </c>
@@ -2429,7 +2540,7 @@
       <c r="D36" s="7">
         <v>1</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="57" t="s">
         <v>70</v>
       </c>
       <c r="F36" s="22">
@@ -2443,7 +2554,7 @@
       </c>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="40"/>
       <c r="C37" s="28"/>
@@ -2452,7 +2563,7 @@
       <c r="H37" s="35"/>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>12</v>
       </c>
@@ -2465,7 +2576,7 @@
       <c r="D38" s="7">
         <v>1</v>
       </c>
-      <c r="E38" s="58" t="s">
+      <c r="E38" s="57" t="s">
         <v>71</v>
       </c>
       <c r="F38" s="4">
@@ -2479,7 +2590,7 @@
       </c>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
         <v>12</v>
       </c>
@@ -2492,7 +2603,7 @@
       <c r="D39" s="28">
         <v>1</v>
       </c>
-      <c r="E39" s="58" t="s">
+      <c r="E39" s="57" t="s">
         <v>71</v>
       </c>
       <c r="F39" s="22">
@@ -2506,7 +2617,7 @@
       </c>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
       <c r="B40" s="40"/>
       <c r="C40" s="28"/>
@@ -2517,7 +2628,7 @@
       <c r="H40" s="33"/>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="42" t="s">
         <v>52</v>
       </c>
@@ -2544,7 +2655,7 @@
       <c r="L41" s="31"/>
       <c r="M41" s="31"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="40"/>
       <c r="C42" s="28"/>
@@ -2559,8 +2670,8 @@
       <c r="L42" s="31"/>
       <c r="M42" s="31"/>
     </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="50" t="s">
+    <row r="43" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="49" t="s">
         <v>55</v>
       </c>
       <c r="B43" t="s">
@@ -2580,8 +2691,8 @@
       <c r="L43" s="31"/>
       <c r="M43" s="31"/>
     </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="50" t="s">
+    <row r="44" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="49" t="s">
         <v>56</v>
       </c>
       <c r="B44" t="s">
@@ -2601,7 +2712,7 @@
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="40"/>
       <c r="C45" s="28"/>
@@ -2616,7 +2727,7 @@
       <c r="L45" s="31"/>
       <c r="M45" s="31"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>77</v>
       </c>
@@ -2635,105 +2746,789 @@
       <c r="F46" t="s">
         <v>72</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" s="60">
+        <v>39</v>
+      </c>
+      <c r="I46" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="J46" s="61">
+        <v>270</v>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="L46" s="26"/>
+    </row>
+    <row r="47" spans="1:13" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="28">
+        <v>1</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G47" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="64">
+        <v>50.070666666666668</v>
+      </c>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="26"/>
+    </row>
+    <row r="48" spans="1:13" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="28">
+        <v>1</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G48" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="64">
+        <v>-144.798</v>
+      </c>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="26"/>
+    </row>
+    <row r="49" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="28">
+        <v>1</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G49" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="45">
+      <c r="H49" s="60">
         <v>1450</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="K46" s="12"/>
-    </row>
-    <row r="47" spans="1:13" ht="14.75" customHeight="1">
-      <c r="A47" s="1" t="s">
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="12"/>
+    </row>
+    <row r="50" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="7">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="B50" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="28">
+        <v>1</v>
+      </c>
+      <c r="E50" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F50" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="26">
-        <v>50.070666666666668</v>
-      </c>
-      <c r="K47" s="12"/>
-    </row>
-    <row r="48" spans="1:13" ht="14.75" customHeight="1">
-      <c r="A48" s="1" t="s">
+      <c r="G50" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H50" s="62">
+        <v>1.9663000000000001E-7</v>
+      </c>
+      <c r="K50" s="12"/>
+    </row>
+    <row r="51" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B48" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="7">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="B51" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="28">
+        <v>1</v>
+      </c>
+      <c r="E51" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F51" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="G48" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="26">
-        <v>-144.798</v>
-      </c>
-      <c r="K48" s="12"/>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="K49" s="12"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="59" t="s">
+      <c r="G51" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H51" s="65">
+        <v>-1.57035E-4</v>
+      </c>
+      <c r="I51" s="63"/>
+      <c r="K51" s="12"/>
+    </row>
+    <row r="52" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="28">
+        <v>1</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52" s="65">
+        <v>3.1441020000000001E-4</v>
+      </c>
+      <c r="I52" s="63"/>
+      <c r="K52" s="12"/>
+    </row>
+    <row r="53" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="28">
+        <v>1</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F53" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H53" s="65">
+        <v>-4.8581210000000001E-6</v>
+      </c>
+      <c r="I53" s="63"/>
+      <c r="K53" s="12"/>
+    </row>
+    <row r="54" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="28">
+        <v>1</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H54" s="65">
+        <v>2.1115559999999999E-7</v>
+      </c>
+      <c r="I54" s="63"/>
+      <c r="K54" s="12"/>
+    </row>
+    <row r="55" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="28">
+        <v>1</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H55" s="62">
+        <v>-69.126630000000006</v>
+      </c>
+      <c r="I55" s="63"/>
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="28">
+        <v>1</v>
+      </c>
+      <c r="E56" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H56" s="62">
+        <v>5.2726729999999999E-2</v>
+      </c>
+      <c r="I56" s="63"/>
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="28">
+        <v>1</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H57" s="62">
+        <v>-7.3390550000000002E-7</v>
+      </c>
+      <c r="I57" s="63"/>
+      <c r="K57" s="12"/>
+    </row>
+    <row r="58" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="28">
+        <v>1</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H58" s="62">
+        <v>525468.80000000005</v>
+      </c>
+      <c r="I58" s="63"/>
+      <c r="K58" s="12"/>
+    </row>
+    <row r="59" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="28">
+        <v>1</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F59" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H59" s="62">
+        <v>7.7548820000000003</v>
+      </c>
+      <c r="I59" s="63"/>
+      <c r="K59" s="12"/>
+    </row>
+    <row r="60" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="28">
+        <v>1</v>
+      </c>
+      <c r="E60" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F60" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H60" s="62">
+        <v>-0.22474089999999999</v>
+      </c>
+      <c r="I60" s="63"/>
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="28">
+        <v>1</v>
+      </c>
+      <c r="E61" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H61" s="62">
+        <v>25.262630000000001</v>
+      </c>
+      <c r="I61" s="63"/>
+      <c r="K61" s="12"/>
+    </row>
+    <row r="62" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="28">
+        <v>1</v>
+      </c>
+      <c r="E62" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H62" s="62">
+        <v>-7.4999999999999993E-5</v>
+      </c>
+      <c r="I62" s="63"/>
+      <c r="K62" s="12"/>
+    </row>
+    <row r="63" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="28">
+        <v>1</v>
+      </c>
+      <c r="E63" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H63" s="62">
+        <v>0</v>
+      </c>
+      <c r="I63" s="63"/>
+      <c r="K63" s="12"/>
+    </row>
+    <row r="64" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="28">
+        <v>1</v>
+      </c>
+      <c r="E64" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H64" s="65">
+        <v>0.28360669999999999</v>
+      </c>
+      <c r="I64" s="63"/>
+      <c r="K64" s="12"/>
+    </row>
+    <row r="65" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="28">
+        <v>1</v>
+      </c>
+      <c r="E65" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H65" s="65">
+        <v>4.5528280000000001E-3</v>
+      </c>
+      <c r="I65" s="63"/>
+      <c r="K65" s="12"/>
+    </row>
+    <row r="66" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="28">
+        <v>1</v>
+      </c>
+      <c r="E66" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F66" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H66" s="65">
+        <v>-1.5026579999999999E-11</v>
+      </c>
+      <c r="I66" s="63"/>
+      <c r="K66" s="12"/>
+    </row>
+    <row r="67" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="28">
+        <v>1</v>
+      </c>
+      <c r="E67" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H67" s="62">
+        <v>-0.97056540000000002</v>
+      </c>
+      <c r="I67" s="63"/>
+      <c r="K67" s="12"/>
+    </row>
+    <row r="68" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="28">
+        <v>1</v>
+      </c>
+      <c r="E68" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F68" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H68" s="62">
+        <v>5.07243E-2</v>
+      </c>
+      <c r="I68" s="63"/>
+      <c r="K68" s="12"/>
+    </row>
+    <row r="69" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="28">
+        <v>1</v>
+      </c>
+      <c r="E69" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F69" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H69" s="62">
+        <v>-3.6618309999999999E-4</v>
+      </c>
+      <c r="I69" s="63"/>
+      <c r="K69" s="12"/>
+    </row>
+    <row r="70" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="28">
+        <v>1</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F70" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H70" s="62">
+        <v>4.9213569999999997E-5</v>
+      </c>
+      <c r="I70" s="63"/>
+      <c r="K70" s="12"/>
+    </row>
+    <row r="71" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="28">
+        <v>1</v>
+      </c>
+      <c r="E71" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F71" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H71" s="62">
+        <v>-9.5700000000000003E-8</v>
+      </c>
+      <c r="I71" s="63"/>
+      <c r="K71" s="12"/>
+    </row>
+    <row r="72" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C72" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="28">
+        <v>1</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F72" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H72" s="62">
+        <v>3.2499999999999998E-6</v>
+      </c>
+      <c r="I72" s="63"/>
+      <c r="K72" s="12"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K73" s="12"/>
+    </row>
+    <row r="74" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="B50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="44">
-        <v>1</v>
-      </c>
-      <c r="E50" s="58" t="s">
+      <c r="B74" t="s">
+        <v>58</v>
+      </c>
+      <c r="C74" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="44">
+        <v>1</v>
+      </c>
+      <c r="E74" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="F50" s="58" t="s">
+      <c r="F74" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="I50" s="31" t="s">
+      <c r="I74" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="K50" s="12"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="K51" s="12"/>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="K52" s="12"/>
+      <c r="K74" s="12"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K75" s="12"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K76" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>